<commit_message>
enclosure for device v2
</commit_message>
<xml_diff>
--- a/pcb/distance_sensor_v2/distance_sensor_v2/Outputs/2023-10-28/bom.xlsx
+++ b/pcb/distance_sensor_v2/distance_sensor_v2/Outputs/2023-10-28/bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\dev\distance_sensor\pcb\distance_sensor_v2\distance_sensor_v2\Outputs\2023-10-28\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7454DA3-7849-416A-801F-2A29D18FA9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FCCCD9-A001-47AF-9B0A-14800A73133D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440" xr2:uid="{2245EF0B-37BA-4207-B279-745AA6C5D67B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
   <si>
     <t>Designator</t>
   </si>
@@ -185,9 +185,6 @@
     <t>N/P Channel MOSFET</t>
   </si>
   <si>
-    <t>R1, R4, R6, R7, R8, R9, R10, R16</t>
-  </si>
-  <si>
     <t>RES 0603_1608</t>
   </si>
   <si>
@@ -197,9 +194,6 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>R2, R13, R15, R17, R18</t>
-  </si>
-  <si>
     <t>R3, R5</t>
   </si>
   <si>
@@ -246,6 +240,9 @@
   </si>
   <si>
     <t>BAT20JFILM</t>
+  </si>
+  <si>
+    <t>R1, R4, R6, R7, R8, R9, R10, R16, R2, R13, R15, R17, R18</t>
   </si>
 </sst>
 </file>
@@ -665,15 +662,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="72.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -811,7 +808,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>22</v>
@@ -938,36 +935,36 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="5">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="5">
-        <v>8</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="5">
-        <v>5</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -978,13 +975,13 @@
         <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -992,72 +989,55 @@
         <v>55</v>
       </c>
       <c r="B19" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B21" s="5">
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="5">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="68" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageMargins left="0.35" right="0.32" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>